<commit_message>
added Liu mac model
</commit_message>
<xml_diff>
--- a/models/library.xlsx
+++ b/models/library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myuva-my.sharepoint.com/personal/jjs3g_virginia_edu/Documents/Documents/research/Netflux2/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="8_{13CC0728-3D84-40EC-BC25-2DCCDD6B4BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B45D14D6-740C-4357-93CE-0750619223C1}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="8_{13CC0728-3D84-40EC-BC25-2DCCDD6B4BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B50D7C9-28DD-4C58-B5DC-750135B421A7}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Model name</t>
   </si>
@@ -83,6 +83,15 @@
   </si>
   <si>
     <t>Zeigler2016_cardiac_fibroblast.png</t>
+  </si>
+  <si>
+    <t>Liu2021_macrophage</t>
+  </si>
+  <si>
+    <t>Liu2021_macrophage.jpeg</t>
+  </si>
+  <si>
+    <t>Liu et al., J. Immunology&lt;br&gt;PMID:33408259&lt;br&gt;&lt;br&gt;Model of the macrophage signaling network.&lt;br&gt;&lt;br&gt;Basic simulations working.</t>
   </si>
 </sst>
 </file>
@@ -636,10 +645,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -677,7 +690,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -783,7 +796,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -925,7 +938,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -933,20 +946,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.6640625" customWidth="1"/>
-    <col min="2" max="2" width="87.3984375" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="1" max="1" width="38.28515625" customWidth="1"/>
+    <col min="2" max="2" width="87.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -957,7 +970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -968,7 +981,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -979,7 +992,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -990,7 +1003,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1001,25 +1014,36 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>